<commit_message>
09.05.2020 (result page completed)
</commit_message>
<xml_diff>
--- a/excel_files/demo/insert_multiple_edit_result.xlsx
+++ b/excel_files/demo/insert_multiple_edit_result.xlsx
@@ -544,9 +544,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -555,6 +552,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,16 +930,16 @@
         <f>IF(OR(G2="",G2&lt;0),"-- N/A --",IF(AND(G2&lt;40,G2&gt;=0),"0.00",IF(AND(G2&lt;45,G2&gt;=40),"2.00",IF(AND(G2&lt;50,G2&gt;=45),"2.25",IF(AND(G2&lt;55,G2&gt;=50),"2.50",IF(AND(G2&lt;60,G2&gt;=55),"2.75",IF(AND(G2&lt;65,G2&gt;=60),"3.00",IF(AND(G2&lt;70,G2&gt;=65),"3.25",IF(AND(G2&lt;75,G2&gt;=70),"3.50",IF(AND(G2&lt;80,G2&gt;=75),"3.75",IF(AND(G2&lt;101,G2&gt;=80),"4.00","-- N/A --")))))))))))</f>
         <v>-- N/A --</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
-      <c r="B3" s="25"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="7" t="s">
         <v>24</v>
       </c>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="25"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="5" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="25"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="7" t="s">
         <v>24</v>
       </c>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="25"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="7" t="s">
         <v>24</v>
       </c>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="7" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="25"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="25"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="9" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="25"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="10" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="25"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="11" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="12" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="7" t="s">
         <v>24</v>
       </c>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="13" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="25"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="7" t="s">
         <v>24</v>
       </c>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="14" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="25"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="7" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="15" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="25"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="16" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="25"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="7" t="s">
         <v>24</v>
       </c>
@@ -1961,7 +1961,7 @@
     </row>
     <row r="17" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="25"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="18" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="25"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="7" t="s">
         <v>24</v>
       </c>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="19" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="25"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="7" t="s">
         <v>24</v>
       </c>
@@ -2180,7 +2180,7 @@
     </row>
     <row r="20" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="25"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="7" t="s">
         <v>24</v>
       </c>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="21" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="7" t="s">
         <v>24</v>
       </c>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="22" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="25"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="7" t="s">
         <v>24</v>
       </c>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="23" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="25"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="7" t="s">
         <v>24</v>
       </c>
@@ -2472,7 +2472,7 @@
     </row>
     <row r="24" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="25"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="25" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="25"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="7" t="s">
         <v>24</v>
       </c>
@@ -2618,7 +2618,7 @@
     </row>
     <row r="26" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="25"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="7" t="s">
         <v>24</v>
       </c>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="27" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="25"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="7" t="s">
         <v>24</v>
       </c>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="28" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="25"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="7" t="s">
         <v>24</v>
       </c>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="29" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="25"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="7" t="s">
         <v>24</v>
       </c>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="30" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="7" t="s">
         <v>24</v>
       </c>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="31" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="25"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="7" t="s">
         <v>24</v>
       </c>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="32" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="25"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
@@ -3129,7 +3129,7 @@
     </row>
     <row r="33" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="25"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="7" t="s">
         <v>24</v>
       </c>
@@ -3202,7 +3202,7 @@
     </row>
     <row r="34" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="25"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="7" t="s">
         <v>24</v>
       </c>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="35" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="25"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="7" t="s">
         <v>24</v>
       </c>
@@ -3348,7 +3348,7 @@
     </row>
     <row r="36" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="25"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="7" t="s">
         <v>24</v>
       </c>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="37" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="25"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="7" t="s">
         <v>24</v>
       </c>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="38" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="25"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="7" t="s">
         <v>24</v>
       </c>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="39" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="25"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="7" t="s">
         <v>24</v>
       </c>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="40" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="25"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="7" t="s">
         <v>24</v>
       </c>
@@ -3713,7 +3713,7 @@
     </row>
     <row r="41" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
-      <c r="B41" s="25"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="7" t="s">
         <v>24</v>
       </c>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="42" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
-      <c r="B42" s="25"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -3859,7 +3859,7 @@
     </row>
     <row r="43" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="25"/>
+      <c r="B43" s="24"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="44" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="25"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="7" t="s">
         <v>24</v>
       </c>
@@ -4005,7 +4005,7 @@
     </row>
     <row r="45" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="25"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
@@ -4078,7 +4078,7 @@
     </row>
     <row r="46" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="25"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="7" t="s">
         <v>24</v>
       </c>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="47" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="25"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="7" t="s">
         <v>24</v>
       </c>
@@ -4224,7 +4224,7 @@
     </row>
     <row r="48" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="B48" s="25"/>
+      <c r="B48" s="24"/>
       <c r="C48" s="7" t="s">
         <v>24</v>
       </c>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="49" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
-      <c r="B49" s="25"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="7" t="s">
         <v>24</v>
       </c>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="50" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
-      <c r="B50" s="25"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="7" t="s">
         <v>24</v>
       </c>
@@ -4443,7 +4443,7 @@
     </row>
     <row r="51" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="25"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="7" t="s">
         <v>24</v>
       </c>
@@ -4516,7 +4516,7 @@
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
-      <c r="B52" s="25"/>
+      <c r="B52" s="24"/>
       <c r="C52" s="7" t="s">
         <v>24</v>
       </c>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="53" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22"/>
-      <c r="B53" s="25"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="7" t="s">
         <v>24</v>
       </c>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="54" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22"/>
-      <c r="B54" s="25"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="7" t="s">
         <v>24</v>
       </c>
@@ -4735,7 +4735,7 @@
     </row>
     <row r="55" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
-      <c r="B55" s="25"/>
+      <c r="B55" s="24"/>
       <c r="C55" s="7" t="s">
         <v>24</v>
       </c>
@@ -4808,7 +4808,7 @@
     </row>
     <row r="56" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22"/>
-      <c r="B56" s="25"/>
+      <c r="B56" s="24"/>
       <c r="C56" s="7" t="s">
         <v>24</v>
       </c>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="57" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="25"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="7" t="s">
         <v>24</v>
       </c>
@@ -4954,7 +4954,7 @@
     </row>
     <row r="58" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
-      <c r="B58" s="25"/>
+      <c r="B58" s="24"/>
       <c r="C58" s="7" t="s">
         <v>24</v>
       </c>
@@ -5027,7 +5027,7 @@
     </row>
     <row r="59" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="25"/>
+      <c r="B59" s="24"/>
       <c r="C59" s="7" t="s">
         <v>24</v>
       </c>
@@ -5100,7 +5100,7 @@
     </row>
     <row r="60" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
-      <c r="B60" s="25"/>
+      <c r="B60" s="24"/>
       <c r="C60" s="7" t="s">
         <v>24</v>
       </c>
@@ -5173,7 +5173,7 @@
     </row>
     <row r="61" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
-      <c r="B61" s="25"/>
+      <c r="B61" s="24"/>
       <c r="C61" s="7" t="s">
         <v>24</v>
       </c>
@@ -5246,7 +5246,7 @@
     </row>
     <row r="62" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
-      <c r="B62" s="25"/>
+      <c r="B62" s="24"/>
       <c r="C62" s="7" t="s">
         <v>24</v>
       </c>
@@ -5319,7 +5319,7 @@
     </row>
     <row r="63" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22"/>
-      <c r="B63" s="25"/>
+      <c r="B63" s="24"/>
       <c r="C63" s="7" t="s">
         <v>24</v>
       </c>
@@ -5392,7 +5392,7 @@
     </row>
     <row r="64" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="22"/>
-      <c r="B64" s="25"/>
+      <c r="B64" s="24"/>
       <c r="C64" s="7" t="s">
         <v>24</v>
       </c>
@@ -5465,7 +5465,7 @@
     </row>
     <row r="65" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="22"/>
-      <c r="B65" s="25"/>
+      <c r="B65" s="24"/>
       <c r="C65" s="7" t="s">
         <v>24</v>
       </c>
@@ -5538,7 +5538,7 @@
     </row>
     <row r="66" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="22"/>
-      <c r="B66" s="25"/>
+      <c r="B66" s="24"/>
       <c r="C66" s="7" t="s">
         <v>24</v>
       </c>
@@ -5611,7 +5611,7 @@
     </row>
     <row r="67" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="22"/>
-      <c r="B67" s="25"/>
+      <c r="B67" s="24"/>
       <c r="C67" s="7" t="s">
         <v>24</v>
       </c>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="68" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22"/>
-      <c r="B68" s="25"/>
+      <c r="B68" s="24"/>
       <c r="C68" s="7" t="s">
         <v>24</v>
       </c>
@@ -5757,7 +5757,7 @@
     </row>
     <row r="69" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="22"/>
-      <c r="B69" s="25"/>
+      <c r="B69" s="24"/>
       <c r="C69" s="7" t="s">
         <v>24</v>
       </c>
@@ -5830,7 +5830,7 @@
     </row>
     <row r="70" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="22"/>
-      <c r="B70" s="25"/>
+      <c r="B70" s="24"/>
       <c r="C70" s="7" t="s">
         <v>24</v>
       </c>
@@ -5903,7 +5903,7 @@
     </row>
     <row r="71" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22"/>
-      <c r="B71" s="25"/>
+      <c r="B71" s="24"/>
       <c r="C71" s="7" t="s">
         <v>24</v>
       </c>
@@ -5976,7 +5976,7 @@
     </row>
     <row r="72" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="22"/>
-      <c r="B72" s="25"/>
+      <c r="B72" s="24"/>
       <c r="C72" s="7" t="s">
         <v>24</v>
       </c>
@@ -6049,7 +6049,7 @@
     </row>
     <row r="73" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="22"/>
-      <c r="B73" s="25"/>
+      <c r="B73" s="24"/>
       <c r="C73" s="7" t="s">
         <v>24</v>
       </c>
@@ -6122,7 +6122,7 @@
     </row>
     <row r="74" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="22"/>
-      <c r="B74" s="25"/>
+      <c r="B74" s="24"/>
       <c r="C74" s="7" t="s">
         <v>24</v>
       </c>
@@ -6195,7 +6195,7 @@
     </row>
     <row r="75" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="22"/>
-      <c r="B75" s="25"/>
+      <c r="B75" s="24"/>
       <c r="C75" s="7" t="s">
         <v>24</v>
       </c>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="76" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
-      <c r="B76" s="25"/>
+      <c r="B76" s="24"/>
       <c r="C76" s="7" t="s">
         <v>24</v>
       </c>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="77" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="22"/>
-      <c r="B77" s="25"/>
+      <c r="B77" s="24"/>
       <c r="C77" s="7" t="s">
         <v>24</v>
       </c>
@@ -6414,7 +6414,7 @@
     </row>
     <row r="78" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="22"/>
-      <c r="B78" s="25"/>
+      <c r="B78" s="24"/>
       <c r="C78" s="7" t="s">
         <v>24</v>
       </c>
@@ -6487,7 +6487,7 @@
     </row>
     <row r="79" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="22"/>
-      <c r="B79" s="25"/>
+      <c r="B79" s="24"/>
       <c r="C79" s="7" t="s">
         <v>24</v>
       </c>
@@ -6560,7 +6560,7 @@
     </row>
     <row r="80" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
-      <c r="B80" s="25"/>
+      <c r="B80" s="24"/>
       <c r="C80" s="7" t="s">
         <v>24</v>
       </c>
@@ -6633,7 +6633,7 @@
     </row>
     <row r="81" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="22"/>
-      <c r="B81" s="25"/>
+      <c r="B81" s="24"/>
       <c r="C81" s="7" t="s">
         <v>24</v>
       </c>
@@ -6706,7 +6706,7 @@
     </row>
     <row r="82" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="22"/>
-      <c r="B82" s="25"/>
+      <c r="B82" s="24"/>
       <c r="C82" s="7" t="s">
         <v>24</v>
       </c>
@@ -6779,7 +6779,7 @@
     </row>
     <row r="83" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
-      <c r="B83" s="25"/>
+      <c r="B83" s="24"/>
       <c r="C83" s="7" t="s">
         <v>24</v>
       </c>
@@ -6852,7 +6852,7 @@
     </row>
     <row r="84" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
-      <c r="B84" s="25"/>
+      <c r="B84" s="24"/>
       <c r="C84" s="7" t="s">
         <v>24</v>
       </c>
@@ -6925,7 +6925,7 @@
     </row>
     <row r="85" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="22"/>
-      <c r="B85" s="25"/>
+      <c r="B85" s="24"/>
       <c r="C85" s="7" t="s">
         <v>24</v>
       </c>
@@ -6998,7 +6998,7 @@
     </row>
     <row r="86" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
-      <c r="B86" s="25"/>
+      <c r="B86" s="24"/>
       <c r="C86" s="7" t="s">
         <v>24</v>
       </c>
@@ -7071,7 +7071,7 @@
     </row>
     <row r="87" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
-      <c r="B87" s="25"/>
+      <c r="B87" s="24"/>
       <c r="C87" s="7" t="s">
         <v>24</v>
       </c>
@@ -7144,7 +7144,7 @@
     </row>
     <row r="88" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="22"/>
-      <c r="B88" s="25"/>
+      <c r="B88" s="24"/>
       <c r="C88" s="7" t="s">
         <v>24</v>
       </c>
@@ -7217,7 +7217,7 @@
     </row>
     <row r="89" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="22"/>
-      <c r="B89" s="25"/>
+      <c r="B89" s="24"/>
       <c r="C89" s="7" t="s">
         <v>24</v>
       </c>
@@ -7290,7 +7290,7 @@
     </row>
     <row r="90" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="22"/>
-      <c r="B90" s="25"/>
+      <c r="B90" s="24"/>
       <c r="C90" s="7" t="s">
         <v>24</v>
       </c>
@@ -7363,7 +7363,7 @@
     </row>
     <row r="91" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="22"/>
-      <c r="B91" s="25"/>
+      <c r="B91" s="24"/>
       <c r="C91" s="7" t="s">
         <v>24</v>
       </c>
@@ -7436,7 +7436,7 @@
     </row>
     <row r="92" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="22"/>
-      <c r="B92" s="25"/>
+      <c r="B92" s="24"/>
       <c r="C92" s="7" t="s">
         <v>24</v>
       </c>
@@ -7509,7 +7509,7 @@
     </row>
     <row r="93" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="22"/>
-      <c r="B93" s="25"/>
+      <c r="B93" s="24"/>
       <c r="C93" s="7" t="s">
         <v>24</v>
       </c>
@@ -7582,7 +7582,7 @@
     </row>
     <row r="94" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="22"/>
-      <c r="B94" s="25"/>
+      <c r="B94" s="24"/>
       <c r="C94" s="7" t="s">
         <v>24</v>
       </c>
@@ -7655,7 +7655,7 @@
     </row>
     <row r="95" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="22"/>
-      <c r="B95" s="25"/>
+      <c r="B95" s="24"/>
       <c r="C95" s="7" t="s">
         <v>24</v>
       </c>
@@ -7728,7 +7728,7 @@
     </row>
     <row r="96" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="22"/>
-      <c r="B96" s="25"/>
+      <c r="B96" s="24"/>
       <c r="C96" s="7" t="s">
         <v>24</v>
       </c>
@@ -7801,7 +7801,7 @@
     </row>
     <row r="97" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="22"/>
-      <c r="B97" s="25"/>
+      <c r="B97" s="24"/>
       <c r="C97" s="7" t="s">
         <v>24</v>
       </c>
@@ -7874,7 +7874,7 @@
     </row>
     <row r="98" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="22"/>
-      <c r="B98" s="25"/>
+      <c r="B98" s="24"/>
       <c r="C98" s="7" t="s">
         <v>24</v>
       </c>
@@ -7947,7 +7947,7 @@
     </row>
     <row r="99" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="22"/>
-      <c r="B99" s="25"/>
+      <c r="B99" s="24"/>
       <c r="C99" s="7" t="s">
         <v>24</v>
       </c>
@@ -8020,7 +8020,7 @@
     </row>
     <row r="100" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="22"/>
-      <c r="B100" s="25"/>
+      <c r="B100" s="24"/>
       <c r="C100" s="7" t="s">
         <v>24</v>
       </c>
@@ -8093,7 +8093,7 @@
     </row>
     <row r="101" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="22"/>
-      <c r="B101" s="25"/>
+      <c r="B101" s="24"/>
       <c r="C101" s="7" t="s">
         <v>24</v>
       </c>
@@ -8166,7 +8166,7 @@
     </row>
     <row r="102" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="22"/>
-      <c r="B102" s="25"/>
+      <c r="B102" s="24"/>
       <c r="C102" s="7" t="s">
         <v>24</v>
       </c>
@@ -8239,7 +8239,7 @@
     </row>
     <row r="103" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="22"/>
-      <c r="B103" s="25"/>
+      <c r="B103" s="24"/>
       <c r="C103" s="7" t="s">
         <v>24</v>
       </c>
@@ -8312,7 +8312,7 @@
     </row>
     <row r="104" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="22"/>
-      <c r="B104" s="25"/>
+      <c r="B104" s="24"/>
       <c r="C104" s="7" t="s">
         <v>24</v>
       </c>
@@ -8385,7 +8385,7 @@
     </row>
     <row r="105" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="22"/>
-      <c r="B105" s="25"/>
+      <c r="B105" s="24"/>
       <c r="C105" s="7" t="s">
         <v>24</v>
       </c>
@@ -8458,7 +8458,7 @@
     </row>
     <row r="106" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="22"/>
-      <c r="B106" s="25"/>
+      <c r="B106" s="24"/>
       <c r="C106" s="7" t="s">
         <v>24</v>
       </c>
@@ -8531,7 +8531,7 @@
     </row>
     <row r="107" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="22"/>
-      <c r="B107" s="25"/>
+      <c r="B107" s="24"/>
       <c r="C107" s="7" t="s">
         <v>24</v>
       </c>
@@ -8604,7 +8604,7 @@
     </row>
     <row r="108" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="22"/>
-      <c r="B108" s="25"/>
+      <c r="B108" s="24"/>
       <c r="C108" s="7" t="s">
         <v>24</v>
       </c>
@@ -8677,7 +8677,7 @@
     </row>
     <row r="109" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="22"/>
-      <c r="B109" s="25"/>
+      <c r="B109" s="24"/>
       <c r="C109" s="7" t="s">
         <v>24</v>
       </c>
@@ -8750,7 +8750,7 @@
     </row>
     <row r="110" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="22"/>
-      <c r="B110" s="25"/>
+      <c r="B110" s="24"/>
       <c r="C110" s="7" t="s">
         <v>24</v>
       </c>
@@ -8823,7 +8823,7 @@
     </row>
     <row r="111" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="22"/>
-      <c r="B111" s="25"/>
+      <c r="B111" s="24"/>
       <c r="C111" s="7" t="s">
         <v>24</v>
       </c>
@@ -8896,7 +8896,7 @@
     </row>
     <row r="112" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="22"/>
-      <c r="B112" s="25"/>
+      <c r="B112" s="24"/>
       <c r="C112" s="7" t="s">
         <v>24</v>
       </c>
@@ -8969,7 +8969,7 @@
     </row>
     <row r="113" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="22"/>
-      <c r="B113" s="25"/>
+      <c r="B113" s="24"/>
       <c r="C113" s="7" t="s">
         <v>24</v>
       </c>
@@ -9042,7 +9042,7 @@
     </row>
     <row r="114" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="22"/>
-      <c r="B114" s="25"/>
+      <c r="B114" s="24"/>
       <c r="C114" s="7" t="s">
         <v>24</v>
       </c>
@@ -9115,7 +9115,7 @@
     </row>
     <row r="115" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="22"/>
-      <c r="B115" s="25"/>
+      <c r="B115" s="24"/>
       <c r="C115" s="7" t="s">
         <v>24</v>
       </c>
@@ -9188,7 +9188,7 @@
     </row>
     <row r="116" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="22"/>
-      <c r="B116" s="25"/>
+      <c r="B116" s="24"/>
       <c r="C116" s="7" t="s">
         <v>24</v>
       </c>
@@ -9261,7 +9261,7 @@
     </row>
     <row r="117" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="22"/>
-      <c r="B117" s="25"/>
+      <c r="B117" s="24"/>
       <c r="C117" s="7" t="s">
         <v>24</v>
       </c>
@@ -9334,7 +9334,7 @@
     </row>
     <row r="118" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="22"/>
-      <c r="B118" s="25"/>
+      <c r="B118" s="24"/>
       <c r="C118" s="7" t="s">
         <v>24</v>
       </c>
@@ -9407,7 +9407,7 @@
     </row>
     <row r="119" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="22"/>
-      <c r="B119" s="25"/>
+      <c r="B119" s="24"/>
       <c r="C119" s="7" t="s">
         <v>24</v>
       </c>
@@ -9480,7 +9480,7 @@
     </row>
     <row r="120" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="22"/>
-      <c r="B120" s="25"/>
+      <c r="B120" s="24"/>
       <c r="C120" s="7" t="s">
         <v>24</v>
       </c>
@@ -9553,7 +9553,7 @@
     </row>
     <row r="121" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="22"/>
-      <c r="B121" s="25"/>
+      <c r="B121" s="24"/>
       <c r="C121" s="7" t="s">
         <v>24</v>
       </c>
@@ -9626,7 +9626,7 @@
     </row>
     <row r="122" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="22"/>
-      <c r="B122" s="25"/>
+      <c r="B122" s="24"/>
       <c r="C122" s="7" t="s">
         <v>24</v>
       </c>
@@ -9699,7 +9699,7 @@
     </row>
     <row r="123" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="22"/>
-      <c r="B123" s="25"/>
+      <c r="B123" s="24"/>
       <c r="C123" s="7" t="s">
         <v>24</v>
       </c>
@@ -9772,7 +9772,7 @@
     </row>
     <row r="124" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="22"/>
-      <c r="B124" s="25"/>
+      <c r="B124" s="24"/>
       <c r="C124" s="7" t="s">
         <v>24</v>
       </c>
@@ -9845,7 +9845,7 @@
     </row>
     <row r="125" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="22"/>
-      <c r="B125" s="25"/>
+      <c r="B125" s="24"/>
       <c r="C125" s="7" t="s">
         <v>24</v>
       </c>
@@ -9918,7 +9918,7 @@
     </row>
     <row r="126" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="22"/>
-      <c r="B126" s="25"/>
+      <c r="B126" s="24"/>
       <c r="C126" s="7" t="s">
         <v>24</v>
       </c>
@@ -9991,7 +9991,7 @@
     </row>
     <row r="127" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="22"/>
-      <c r="B127" s="25"/>
+      <c r="B127" s="24"/>
       <c r="C127" s="7" t="s">
         <v>24</v>
       </c>
@@ -10064,7 +10064,7 @@
     </row>
     <row r="128" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="22"/>
-      <c r="B128" s="25"/>
+      <c r="B128" s="24"/>
       <c r="C128" s="7" t="s">
         <v>24</v>
       </c>
@@ -10137,7 +10137,7 @@
     </row>
     <row r="129" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="22"/>
-      <c r="B129" s="25"/>
+      <c r="B129" s="24"/>
       <c r="C129" s="7" t="s">
         <v>24</v>
       </c>
@@ -10210,7 +10210,7 @@
     </row>
     <row r="130" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="22"/>
-      <c r="B130" s="25"/>
+      <c r="B130" s="24"/>
       <c r="C130" s="7" t="s">
         <v>24</v>
       </c>
@@ -10283,7 +10283,7 @@
     </row>
     <row r="131" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A131" s="22"/>
-      <c r="B131" s="25"/>
+      <c r="B131" s="24"/>
       <c r="C131" s="7" t="s">
         <v>24</v>
       </c>
@@ -10356,7 +10356,7 @@
     </row>
     <row r="132" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="22"/>
-      <c r="B132" s="25"/>
+      <c r="B132" s="24"/>
       <c r="C132" s="7" t="s">
         <v>24</v>
       </c>
@@ -10429,7 +10429,7 @@
     </row>
     <row r="133" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="22"/>
-      <c r="B133" s="25"/>
+      <c r="B133" s="24"/>
       <c r="C133" s="7" t="s">
         <v>24</v>
       </c>
@@ -10502,7 +10502,7 @@
     </row>
     <row r="134" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="22"/>
-      <c r="B134" s="25"/>
+      <c r="B134" s="24"/>
       <c r="C134" s="7" t="s">
         <v>24</v>
       </c>
@@ -10575,7 +10575,7 @@
     </row>
     <row r="135" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="22"/>
-      <c r="B135" s="25"/>
+      <c r="B135" s="24"/>
       <c r="C135" s="7" t="s">
         <v>24</v>
       </c>
@@ -10648,7 +10648,7 @@
     </row>
     <row r="136" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="22"/>
-      <c r="B136" s="25"/>
+      <c r="B136" s="24"/>
       <c r="C136" s="7" t="s">
         <v>24</v>
       </c>
@@ -10721,7 +10721,7 @@
     </row>
     <row r="137" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="22"/>
-      <c r="B137" s="25"/>
+      <c r="B137" s="24"/>
       <c r="C137" s="7" t="s">
         <v>24</v>
       </c>
@@ -10794,7 +10794,7 @@
     </row>
     <row r="138" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="22"/>
-      <c r="B138" s="25"/>
+      <c r="B138" s="24"/>
       <c r="C138" s="7" t="s">
         <v>24</v>
       </c>
@@ -10867,7 +10867,7 @@
     </row>
     <row r="139" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A139" s="22"/>
-      <c r="B139" s="25"/>
+      <c r="B139" s="24"/>
       <c r="C139" s="7" t="s">
         <v>24</v>
       </c>
@@ -10940,7 +10940,7 @@
     </row>
     <row r="140" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="22"/>
-      <c r="B140" s="25"/>
+      <c r="B140" s="24"/>
       <c r="C140" s="7" t="s">
         <v>24</v>
       </c>
@@ -11013,7 +11013,7 @@
     </row>
     <row r="141" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="22"/>
-      <c r="B141" s="25"/>
+      <c r="B141" s="24"/>
       <c r="C141" s="7" t="s">
         <v>24</v>
       </c>
@@ -11086,7 +11086,7 @@
     </row>
     <row r="142" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="22"/>
-      <c r="B142" s="25"/>
+      <c r="B142" s="24"/>
       <c r="C142" s="7" t="s">
         <v>24</v>
       </c>
@@ -11159,7 +11159,7 @@
     </row>
     <row r="143" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="22"/>
-      <c r="B143" s="25"/>
+      <c r="B143" s="24"/>
       <c r="C143" s="7" t="s">
         <v>24</v>
       </c>
@@ -11232,7 +11232,7 @@
     </row>
     <row r="144" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="22"/>
-      <c r="B144" s="25"/>
+      <c r="B144" s="24"/>
       <c r="C144" s="7" t="s">
         <v>24</v>
       </c>
@@ -11305,7 +11305,7 @@
     </row>
     <row r="145" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A145" s="22"/>
-      <c r="B145" s="25"/>
+      <c r="B145" s="24"/>
       <c r="C145" s="7" t="s">
         <v>24</v>
       </c>
@@ -11378,7 +11378,7 @@
     </row>
     <row r="146" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="22"/>
-      <c r="B146" s="25"/>
+      <c r="B146" s="24"/>
       <c r="C146" s="7" t="s">
         <v>24</v>
       </c>
@@ -11451,7 +11451,7 @@
     </row>
     <row r="147" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A147" s="22"/>
-      <c r="B147" s="25"/>
+      <c r="B147" s="24"/>
       <c r="C147" s="7" t="s">
         <v>24</v>
       </c>
@@ -11524,7 +11524,7 @@
     </row>
     <row r="148" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A148" s="22"/>
-      <c r="B148" s="25"/>
+      <c r="B148" s="24"/>
       <c r="C148" s="7" t="s">
         <v>24</v>
       </c>
@@ -11597,7 +11597,7 @@
     </row>
     <row r="149" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A149" s="22"/>
-      <c r="B149" s="25"/>
+      <c r="B149" s="24"/>
       <c r="C149" s="7" t="s">
         <v>24</v>
       </c>
@@ -11670,7 +11670,7 @@
     </row>
     <row r="150" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="22"/>
-      <c r="B150" s="25"/>
+      <c r="B150" s="24"/>
       <c r="C150" s="7" t="s">
         <v>24</v>
       </c>
@@ -11743,7 +11743,7 @@
     </row>
     <row r="151" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A151" s="22"/>
-      <c r="B151" s="25"/>
+      <c r="B151" s="24"/>
       <c r="C151" s="7" t="s">
         <v>24</v>
       </c>
@@ -11816,7 +11816,7 @@
     </row>
     <row r="152" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A152" s="22"/>
-      <c r="B152" s="25"/>
+      <c r="B152" s="24"/>
       <c r="C152" s="7" t="s">
         <v>24</v>
       </c>
@@ -11889,7 +11889,7 @@
     </row>
     <row r="153" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="22"/>
-      <c r="B153" s="25"/>
+      <c r="B153" s="24"/>
       <c r="C153" s="7" t="s">
         <v>24</v>
       </c>
@@ -11962,7 +11962,7 @@
     </row>
     <row r="154" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A154" s="22"/>
-      <c r="B154" s="25"/>
+      <c r="B154" s="24"/>
       <c r="C154" s="7" t="s">
         <v>24</v>
       </c>
@@ -12035,7 +12035,7 @@
     </row>
     <row r="155" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A155" s="22"/>
-      <c r="B155" s="25"/>
+      <c r="B155" s="24"/>
       <c r="C155" s="7" t="s">
         <v>24</v>
       </c>
@@ -12108,7 +12108,7 @@
     </row>
     <row r="156" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="22"/>
-      <c r="B156" s="25"/>
+      <c r="B156" s="24"/>
       <c r="C156" s="7" t="s">
         <v>24</v>
       </c>
@@ -12181,7 +12181,7 @@
     </row>
     <row r="157" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A157" s="22"/>
-      <c r="B157" s="25"/>
+      <c r="B157" s="24"/>
       <c r="C157" s="7" t="s">
         <v>24</v>
       </c>
@@ -12254,7 +12254,7 @@
     </row>
     <row r="158" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A158" s="22"/>
-      <c r="B158" s="25"/>
+      <c r="B158" s="24"/>
       <c r="C158" s="7" t="s">
         <v>24</v>
       </c>
@@ -12327,7 +12327,7 @@
     </row>
     <row r="159" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A159" s="22"/>
-      <c r="B159" s="25"/>
+      <c r="B159" s="24"/>
       <c r="C159" s="7" t="s">
         <v>24</v>
       </c>
@@ -12400,7 +12400,7 @@
     </row>
     <row r="160" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A160" s="22"/>
-      <c r="B160" s="25"/>
+      <c r="B160" s="24"/>
       <c r="C160" s="7" t="s">
         <v>24</v>
       </c>
@@ -12473,7 +12473,7 @@
     </row>
     <row r="161" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="22"/>
-      <c r="B161" s="25"/>
+      <c r="B161" s="24"/>
       <c r="C161" s="7" t="s">
         <v>24</v>
       </c>
@@ -12546,7 +12546,7 @@
     </row>
     <row r="162" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="22"/>
-      <c r="B162" s="25"/>
+      <c r="B162" s="24"/>
       <c r="C162" s="7" t="s">
         <v>24</v>
       </c>
@@ -12619,7 +12619,7 @@
     </row>
     <row r="163" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A163" s="22"/>
-      <c r="B163" s="25"/>
+      <c r="B163" s="24"/>
       <c r="C163" s="7" t="s">
         <v>24</v>
       </c>
@@ -12692,7 +12692,7 @@
     </row>
     <row r="164" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="22"/>
-      <c r="B164" s="25"/>
+      <c r="B164" s="24"/>
       <c r="C164" s="7" t="s">
         <v>24</v>
       </c>
@@ -12765,7 +12765,7 @@
     </row>
     <row r="165" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="22"/>
-      <c r="B165" s="25"/>
+      <c r="B165" s="24"/>
       <c r="C165" s="7" t="s">
         <v>24</v>
       </c>
@@ -12838,7 +12838,7 @@
     </row>
     <row r="166" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="22"/>
-      <c r="B166" s="25"/>
+      <c r="B166" s="24"/>
       <c r="C166" s="7" t="s">
         <v>24</v>
       </c>
@@ -12911,7 +12911,7 @@
     </row>
     <row r="167" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A167" s="22"/>
-      <c r="B167" s="25"/>
+      <c r="B167" s="24"/>
       <c r="C167" s="7" t="s">
         <v>24</v>
       </c>
@@ -12984,7 +12984,7 @@
     </row>
     <row r="168" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="22"/>
-      <c r="B168" s="25"/>
+      <c r="B168" s="24"/>
       <c r="C168" s="7" t="s">
         <v>24</v>
       </c>
@@ -13057,7 +13057,7 @@
     </row>
     <row r="169" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A169" s="22"/>
-      <c r="B169" s="25"/>
+      <c r="B169" s="24"/>
       <c r="C169" s="7" t="s">
         <v>24</v>
       </c>
@@ -13130,7 +13130,7 @@
     </row>
     <row r="170" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A170" s="22"/>
-      <c r="B170" s="25"/>
+      <c r="B170" s="24"/>
       <c r="C170" s="7" t="s">
         <v>24</v>
       </c>
@@ -13203,7 +13203,7 @@
     </row>
     <row r="171" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="22"/>
-      <c r="B171" s="25"/>
+      <c r="B171" s="24"/>
       <c r="C171" s="7" t="s">
         <v>24</v>
       </c>
@@ -13276,7 +13276,7 @@
     </row>
     <row r="172" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A172" s="22"/>
-      <c r="B172" s="25"/>
+      <c r="B172" s="24"/>
       <c r="C172" s="7" t="s">
         <v>24</v>
       </c>
@@ -13349,7 +13349,7 @@
     </row>
     <row r="173" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A173" s="22"/>
-      <c r="B173" s="25"/>
+      <c r="B173" s="24"/>
       <c r="C173" s="7" t="s">
         <v>24</v>
       </c>
@@ -13422,7 +13422,7 @@
     </row>
     <row r="174" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A174" s="22"/>
-      <c r="B174" s="25"/>
+      <c r="B174" s="24"/>
       <c r="C174" s="7" t="s">
         <v>24</v>
       </c>
@@ -13495,7 +13495,7 @@
     </row>
     <row r="175" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A175" s="22"/>
-      <c r="B175" s="25"/>
+      <c r="B175" s="24"/>
       <c r="C175" s="7" t="s">
         <v>24</v>
       </c>
@@ -13568,7 +13568,7 @@
     </row>
     <row r="176" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A176" s="22"/>
-      <c r="B176" s="25"/>
+      <c r="B176" s="24"/>
       <c r="C176" s="7" t="s">
         <v>24</v>
       </c>
@@ -13641,7 +13641,7 @@
     </row>
     <row r="177" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A177" s="22"/>
-      <c r="B177" s="25"/>
+      <c r="B177" s="24"/>
       <c r="C177" s="7" t="s">
         <v>24</v>
       </c>
@@ -13714,7 +13714,7 @@
     </row>
     <row r="178" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A178" s="22"/>
-      <c r="B178" s="25"/>
+      <c r="B178" s="24"/>
       <c r="C178" s="7" t="s">
         <v>24</v>
       </c>
@@ -13787,7 +13787,7 @@
     </row>
     <row r="179" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A179" s="22"/>
-      <c r="B179" s="25"/>
+      <c r="B179" s="24"/>
       <c r="C179" s="7" t="s">
         <v>24</v>
       </c>
@@ -13860,7 +13860,7 @@
     </row>
     <row r="180" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A180" s="22"/>
-      <c r="B180" s="25"/>
+      <c r="B180" s="24"/>
       <c r="C180" s="7" t="s">
         <v>24</v>
       </c>
@@ -13933,7 +13933,7 @@
     </row>
     <row r="181" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A181" s="22"/>
-      <c r="B181" s="25"/>
+      <c r="B181" s="24"/>
       <c r="C181" s="7" t="s">
         <v>24</v>
       </c>
@@ -14006,7 +14006,7 @@
     </row>
     <row r="182" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A182" s="22"/>
-      <c r="B182" s="25"/>
+      <c r="B182" s="24"/>
       <c r="C182" s="7" t="s">
         <v>24</v>
       </c>
@@ -14079,7 +14079,7 @@
     </row>
     <row r="183" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A183" s="22"/>
-      <c r="B183" s="25"/>
+      <c r="B183" s="24"/>
       <c r="C183" s="7" t="s">
         <v>24</v>
       </c>
@@ -14152,7 +14152,7 @@
     </row>
     <row r="184" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A184" s="22"/>
-      <c r="B184" s="25"/>
+      <c r="B184" s="24"/>
       <c r="C184" s="7" t="s">
         <v>24</v>
       </c>
@@ -14225,7 +14225,7 @@
     </row>
     <row r="185" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A185" s="22"/>
-      <c r="B185" s="25"/>
+      <c r="B185" s="24"/>
       <c r="C185" s="7" t="s">
         <v>24</v>
       </c>
@@ -14298,7 +14298,7 @@
     </row>
     <row r="186" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A186" s="22"/>
-      <c r="B186" s="25"/>
+      <c r="B186" s="24"/>
       <c r="C186" s="7" t="s">
         <v>24</v>
       </c>
@@ -14371,7 +14371,7 @@
     </row>
     <row r="187" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A187" s="22"/>
-      <c r="B187" s="25"/>
+      <c r="B187" s="24"/>
       <c r="C187" s="7" t="s">
         <v>24</v>
       </c>
@@ -14444,7 +14444,7 @@
     </row>
     <row r="188" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A188" s="22"/>
-      <c r="B188" s="25"/>
+      <c r="B188" s="24"/>
       <c r="C188" s="7" t="s">
         <v>24</v>
       </c>
@@ -14517,7 +14517,7 @@
     </row>
     <row r="189" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A189" s="22"/>
-      <c r="B189" s="25"/>
+      <c r="B189" s="24"/>
       <c r="C189" s="7" t="s">
         <v>24</v>
       </c>
@@ -14590,7 +14590,7 @@
     </row>
     <row r="190" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A190" s="22"/>
-      <c r="B190" s="25"/>
+      <c r="B190" s="24"/>
       <c r="C190" s="7" t="s">
         <v>24</v>
       </c>
@@ -14663,7 +14663,7 @@
     </row>
     <row r="191" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A191" s="22"/>
-      <c r="B191" s="25"/>
+      <c r="B191" s="24"/>
       <c r="C191" s="7" t="s">
         <v>24</v>
       </c>
@@ -14736,7 +14736,7 @@
     </row>
     <row r="192" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="22"/>
-      <c r="B192" s="25"/>
+      <c r="B192" s="24"/>
       <c r="C192" s="7" t="s">
         <v>24</v>
       </c>
@@ -14809,7 +14809,7 @@
     </row>
     <row r="193" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="22"/>
-      <c r="B193" s="25"/>
+      <c r="B193" s="24"/>
       <c r="C193" s="7" t="s">
         <v>24</v>
       </c>
@@ -14882,7 +14882,7 @@
     </row>
     <row r="194" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A194" s="22"/>
-      <c r="B194" s="25"/>
+      <c r="B194" s="24"/>
       <c r="C194" s="7" t="s">
         <v>24</v>
       </c>
@@ -14955,7 +14955,7 @@
     </row>
     <row r="195" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A195" s="22"/>
-      <c r="B195" s="25"/>
+      <c r="B195" s="24"/>
       <c r="C195" s="7" t="s">
         <v>24</v>
       </c>
@@ -15028,7 +15028,7 @@
     </row>
     <row r="196" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A196" s="22"/>
-      <c r="B196" s="25"/>
+      <c r="B196" s="24"/>
       <c r="C196" s="7" t="s">
         <v>24</v>
       </c>
@@ -15101,7 +15101,7 @@
     </row>
     <row r="197" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A197" s="22"/>
-      <c r="B197" s="25"/>
+      <c r="B197" s="24"/>
       <c r="C197" s="7" t="s">
         <v>24</v>
       </c>
@@ -15174,7 +15174,7 @@
     </row>
     <row r="198" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A198" s="22"/>
-      <c r="B198" s="25"/>
+      <c r="B198" s="24"/>
       <c r="C198" s="7" t="s">
         <v>24</v>
       </c>
@@ -15247,7 +15247,7 @@
     </row>
     <row r="199" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A199" s="22"/>
-      <c r="B199" s="25"/>
+      <c r="B199" s="24"/>
       <c r="C199" s="7" t="s">
         <v>24</v>
       </c>
@@ -15320,7 +15320,7 @@
     </row>
     <row r="200" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A200" s="22"/>
-      <c r="B200" s="25"/>
+      <c r="B200" s="24"/>
       <c r="C200" s="7" t="s">
         <v>24</v>
       </c>
@@ -15393,7 +15393,7 @@
     </row>
     <row r="201" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A201" s="22"/>
-      <c r="B201" s="25"/>
+      <c r="B201" s="24"/>
       <c r="C201" s="7" t="s">
         <v>24</v>
       </c>
@@ -15466,7 +15466,7 @@
     </row>
     <row r="202" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A202" s="22"/>
-      <c r="B202" s="25"/>
+      <c r="B202" s="24"/>
       <c r="C202" s="7" t="s">
         <v>24</v>
       </c>
@@ -15539,7 +15539,7 @@
     </row>
     <row r="203" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A203" s="22"/>
-      <c r="B203" s="25"/>
+      <c r="B203" s="24"/>
       <c r="C203" s="7" t="s">
         <v>24</v>
       </c>
@@ -15612,7 +15612,7 @@
     </row>
     <row r="204" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A204" s="22"/>
-      <c r="B204" s="25"/>
+      <c r="B204" s="24"/>
       <c r="C204" s="7" t="s">
         <v>24</v>
       </c>
@@ -15685,7 +15685,7 @@
     </row>
     <row r="205" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A205" s="22"/>
-      <c r="B205" s="25"/>
+      <c r="B205" s="24"/>
       <c r="C205" s="7" t="s">
         <v>24</v>
       </c>
@@ -15758,7 +15758,7 @@
     </row>
     <row r="206" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A206" s="22"/>
-      <c r="B206" s="25"/>
+      <c r="B206" s="24"/>
       <c r="C206" s="7" t="s">
         <v>24</v>
       </c>
@@ -15831,7 +15831,7 @@
     </row>
     <row r="207" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="22"/>
-      <c r="B207" s="25"/>
+      <c r="B207" s="24"/>
       <c r="C207" s="7" t="s">
         <v>24</v>
       </c>
@@ -15904,7 +15904,7 @@
     </row>
     <row r="208" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A208" s="22"/>
-      <c r="B208" s="25"/>
+      <c r="B208" s="24"/>
       <c r="C208" s="7" t="s">
         <v>24</v>
       </c>
@@ -15977,7 +15977,7 @@
     </row>
     <row r="209" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A209" s="22"/>
-      <c r="B209" s="25"/>
+      <c r="B209" s="24"/>
       <c r="C209" s="7" t="s">
         <v>24</v>
       </c>
@@ -16050,7 +16050,7 @@
     </row>
     <row r="210" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A210" s="22"/>
-      <c r="B210" s="25"/>
+      <c r="B210" s="24"/>
       <c r="C210" s="7" t="s">
         <v>24</v>
       </c>
@@ -16123,7 +16123,7 @@
     </row>
     <row r="211" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A211" s="22"/>
-      <c r="B211" s="25"/>
+      <c r="B211" s="24"/>
       <c r="C211" s="7" t="s">
         <v>24</v>
       </c>
@@ -16196,7 +16196,7 @@
     </row>
     <row r="212" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A212" s="22"/>
-      <c r="B212" s="25"/>
+      <c r="B212" s="24"/>
       <c r="C212" s="7" t="s">
         <v>24</v>
       </c>
@@ -16269,7 +16269,7 @@
     </row>
     <row r="213" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A213" s="22"/>
-      <c r="B213" s="25"/>
+      <c r="B213" s="24"/>
       <c r="C213" s="7" t="s">
         <v>24</v>
       </c>
@@ -16342,7 +16342,7 @@
     </row>
     <row r="214" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A214" s="22"/>
-      <c r="B214" s="25"/>
+      <c r="B214" s="24"/>
       <c r="C214" s="7" t="s">
         <v>24</v>
       </c>
@@ -16415,7 +16415,7 @@
     </row>
     <row r="215" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A215" s="22"/>
-      <c r="B215" s="25"/>
+      <c r="B215" s="24"/>
       <c r="C215" s="7" t="s">
         <v>24</v>
       </c>
@@ -16488,7 +16488,7 @@
     </row>
     <row r="216" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A216" s="22"/>
-      <c r="B216" s="25"/>
+      <c r="B216" s="24"/>
       <c r="C216" s="7" t="s">
         <v>24</v>
       </c>
@@ -16561,7 +16561,7 @@
     </row>
     <row r="217" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A217" s="22"/>
-      <c r="B217" s="25"/>
+      <c r="B217" s="24"/>
       <c r="C217" s="7" t="s">
         <v>24</v>
       </c>
@@ -16634,7 +16634,7 @@
     </row>
     <row r="218" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A218" s="22"/>
-      <c r="B218" s="25"/>
+      <c r="B218" s="24"/>
       <c r="C218" s="7" t="s">
         <v>24</v>
       </c>
@@ -16707,7 +16707,7 @@
     </row>
     <row r="219" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A219" s="22"/>
-      <c r="B219" s="25"/>
+      <c r="B219" s="24"/>
       <c r="C219" s="7" t="s">
         <v>24</v>
       </c>
@@ -16780,7 +16780,7 @@
     </row>
     <row r="220" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A220" s="22"/>
-      <c r="B220" s="25"/>
+      <c r="B220" s="24"/>
       <c r="C220" s="7" t="s">
         <v>24</v>
       </c>
@@ -16853,7 +16853,7 @@
     </row>
     <row r="221" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A221" s="22"/>
-      <c r="B221" s="25"/>
+      <c r="B221" s="24"/>
       <c r="C221" s="7" t="s">
         <v>24</v>
       </c>
@@ -16926,7 +16926,7 @@
     </row>
     <row r="222" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A222" s="22"/>
-      <c r="B222" s="25"/>
+      <c r="B222" s="24"/>
       <c r="C222" s="7" t="s">
         <v>24</v>
       </c>
@@ -16999,7 +16999,7 @@
     </row>
     <row r="223" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A223" s="22"/>
-      <c r="B223" s="25"/>
+      <c r="B223" s="24"/>
       <c r="C223" s="7" t="s">
         <v>24</v>
       </c>
@@ -17072,7 +17072,7 @@
     </row>
     <row r="224" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A224" s="22"/>
-      <c r="B224" s="25"/>
+      <c r="B224" s="24"/>
       <c r="C224" s="7" t="s">
         <v>24</v>
       </c>
@@ -17145,7 +17145,7 @@
     </row>
     <row r="225" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A225" s="22"/>
-      <c r="B225" s="25"/>
+      <c r="B225" s="24"/>
       <c r="C225" s="7" t="s">
         <v>24</v>
       </c>
@@ -17218,7 +17218,7 @@
     </row>
     <row r="226" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A226" s="22"/>
-      <c r="B226" s="25"/>
+      <c r="B226" s="24"/>
       <c r="C226" s="7" t="s">
         <v>24</v>
       </c>
@@ -17291,7 +17291,7 @@
     </row>
     <row r="227" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A227" s="22"/>
-      <c r="B227" s="25"/>
+      <c r="B227" s="24"/>
       <c r="C227" s="7" t="s">
         <v>24</v>
       </c>
@@ -17364,7 +17364,7 @@
     </row>
     <row r="228" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A228" s="22"/>
-      <c r="B228" s="25"/>
+      <c r="B228" s="24"/>
       <c r="C228" s="7" t="s">
         <v>24</v>
       </c>
@@ -17437,7 +17437,7 @@
     </row>
     <row r="229" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A229" s="22"/>
-      <c r="B229" s="25"/>
+      <c r="B229" s="24"/>
       <c r="C229" s="7" t="s">
         <v>24</v>
       </c>
@@ -17510,7 +17510,7 @@
     </row>
     <row r="230" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A230" s="22"/>
-      <c r="B230" s="25"/>
+      <c r="B230" s="24"/>
       <c r="C230" s="7" t="s">
         <v>24</v>
       </c>
@@ -17583,7 +17583,7 @@
     </row>
     <row r="231" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A231" s="22"/>
-      <c r="B231" s="25"/>
+      <c r="B231" s="24"/>
       <c r="C231" s="7" t="s">
         <v>24</v>
       </c>
@@ -17656,7 +17656,7 @@
     </row>
     <row r="232" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A232" s="22"/>
-      <c r="B232" s="25"/>
+      <c r="B232" s="24"/>
       <c r="C232" s="7" t="s">
         <v>24</v>
       </c>
@@ -17729,7 +17729,7 @@
     </row>
     <row r="233" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A233" s="22"/>
-      <c r="B233" s="25"/>
+      <c r="B233" s="24"/>
       <c r="C233" s="7" t="s">
         <v>24</v>
       </c>
@@ -17802,7 +17802,7 @@
     </row>
     <row r="234" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A234" s="22"/>
-      <c r="B234" s="25"/>
+      <c r="B234" s="24"/>
       <c r="C234" s="7" t="s">
         <v>24</v>
       </c>
@@ -17875,7 +17875,7 @@
     </row>
     <row r="235" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A235" s="22"/>
-      <c r="B235" s="25"/>
+      <c r="B235" s="24"/>
       <c r="C235" s="7" t="s">
         <v>24</v>
       </c>
@@ -17948,7 +17948,7 @@
     </row>
     <row r="236" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A236" s="22"/>
-      <c r="B236" s="25"/>
+      <c r="B236" s="24"/>
       <c r="C236" s="7" t="s">
         <v>24</v>
       </c>
@@ -18021,7 +18021,7 @@
     </row>
     <row r="237" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A237" s="22"/>
-      <c r="B237" s="25"/>
+      <c r="B237" s="24"/>
       <c r="C237" s="7" t="s">
         <v>24</v>
       </c>
@@ -18094,7 +18094,7 @@
     </row>
     <row r="238" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A238" s="22"/>
-      <c r="B238" s="25"/>
+      <c r="B238" s="24"/>
       <c r="C238" s="7" t="s">
         <v>24</v>
       </c>
@@ -18167,7 +18167,7 @@
     </row>
     <row r="239" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A239" s="22"/>
-      <c r="B239" s="25"/>
+      <c r="B239" s="24"/>
       <c r="C239" s="7" t="s">
         <v>24</v>
       </c>
@@ -18240,7 +18240,7 @@
     </row>
     <row r="240" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A240" s="22"/>
-      <c r="B240" s="25"/>
+      <c r="B240" s="24"/>
       <c r="C240" s="7" t="s">
         <v>24</v>
       </c>
@@ -18313,7 +18313,7 @@
     </row>
     <row r="241" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A241" s="22"/>
-      <c r="B241" s="25"/>
+      <c r="B241" s="24"/>
       <c r="C241" s="7" t="s">
         <v>24</v>
       </c>
@@ -18386,7 +18386,7 @@
     </row>
     <row r="242" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A242" s="22"/>
-      <c r="B242" s="25"/>
+      <c r="B242" s="24"/>
       <c r="C242" s="7" t="s">
         <v>24</v>
       </c>
@@ -18459,7 +18459,7 @@
     </row>
     <row r="243" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A243" s="22"/>
-      <c r="B243" s="25"/>
+      <c r="B243" s="24"/>
       <c r="C243" s="7" t="s">
         <v>24</v>
       </c>
@@ -18532,7 +18532,7 @@
     </row>
     <row r="244" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A244" s="22"/>
-      <c r="B244" s="25"/>
+      <c r="B244" s="24"/>
       <c r="C244" s="7" t="s">
         <v>24</v>
       </c>
@@ -18605,7 +18605,7 @@
     </row>
     <row r="245" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A245" s="22"/>
-      <c r="B245" s="25"/>
+      <c r="B245" s="24"/>
       <c r="C245" s="7" t="s">
         <v>24</v>
       </c>
@@ -18678,7 +18678,7 @@
     </row>
     <row r="246" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A246" s="22"/>
-      <c r="B246" s="25"/>
+      <c r="B246" s="24"/>
       <c r="C246" s="7" t="s">
         <v>24</v>
       </c>
@@ -18751,7 +18751,7 @@
     </row>
     <row r="247" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A247" s="22"/>
-      <c r="B247" s="25"/>
+      <c r="B247" s="24"/>
       <c r="C247" s="7" t="s">
         <v>24</v>
       </c>
@@ -18824,7 +18824,7 @@
     </row>
     <row r="248" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A248" s="22"/>
-      <c r="B248" s="25"/>
+      <c r="B248" s="24"/>
       <c r="C248" s="7" t="s">
         <v>24</v>
       </c>
@@ -18897,7 +18897,7 @@
     </row>
     <row r="249" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A249" s="22"/>
-      <c r="B249" s="25"/>
+      <c r="B249" s="24"/>
       <c r="C249" s="7" t="s">
         <v>24</v>
       </c>
@@ -18970,7 +18970,7 @@
     </row>
     <row r="250" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A250" s="22"/>
-      <c r="B250" s="25"/>
+      <c r="B250" s="24"/>
       <c r="C250" s="7" t="s">
         <v>24</v>
       </c>
@@ -19043,7 +19043,7 @@
     </row>
     <row r="251" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A251" s="22"/>
-      <c r="B251" s="25"/>
+      <c r="B251" s="24"/>
       <c r="C251" s="7" t="s">
         <v>24</v>
       </c>
@@ -19116,7 +19116,7 @@
     </row>
     <row r="252" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A252" s="22"/>
-      <c r="B252" s="25"/>
+      <c r="B252" s="24"/>
       <c r="C252" s="7" t="s">
         <v>24</v>
       </c>
@@ -19189,7 +19189,7 @@
     </row>
     <row r="253" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A253" s="22"/>
-      <c r="B253" s="25"/>
+      <c r="B253" s="24"/>
       <c r="C253" s="7" t="s">
         <v>24</v>
       </c>
@@ -19262,7 +19262,7 @@
     </row>
     <row r="254" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A254" s="22"/>
-      <c r="B254" s="25"/>
+      <c r="B254" s="24"/>
       <c r="C254" s="7" t="s">
         <v>24</v>
       </c>
@@ -19335,7 +19335,7 @@
     </row>
     <row r="255" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A255" s="22"/>
-      <c r="B255" s="25"/>
+      <c r="B255" s="24"/>
       <c r="C255" s="7" t="s">
         <v>24</v>
       </c>
@@ -19408,7 +19408,7 @@
     </row>
     <row r="256" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A256" s="22"/>
-      <c r="B256" s="25"/>
+      <c r="B256" s="24"/>
       <c r="C256" s="7" t="s">
         <v>24</v>
       </c>
@@ -19481,7 +19481,7 @@
     </row>
     <row r="257" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A257" s="22"/>
-      <c r="B257" s="25"/>
+      <c r="B257" s="24"/>
       <c r="C257" s="7" t="s">
         <v>24</v>
       </c>
@@ -19554,7 +19554,7 @@
     </row>
     <row r="258" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A258" s="22"/>
-      <c r="B258" s="25"/>
+      <c r="B258" s="24"/>
       <c r="C258" s="7" t="s">
         <v>24</v>
       </c>
@@ -19627,7 +19627,7 @@
     </row>
     <row r="259" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A259" s="22"/>
-      <c r="B259" s="25"/>
+      <c r="B259" s="24"/>
       <c r="C259" s="7" t="s">
         <v>24</v>
       </c>
@@ -19700,7 +19700,7 @@
     </row>
     <row r="260" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A260" s="22"/>
-      <c r="B260" s="25"/>
+      <c r="B260" s="24"/>
       <c r="C260" s="7" t="s">
         <v>24</v>
       </c>
@@ -19773,7 +19773,7 @@
     </row>
     <row r="261" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A261" s="22"/>
-      <c r="B261" s="25"/>
+      <c r="B261" s="24"/>
       <c r="C261" s="7" t="s">
         <v>24</v>
       </c>
@@ -19846,7 +19846,7 @@
     </row>
     <row r="262" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A262" s="22"/>
-      <c r="B262" s="25"/>
+      <c r="B262" s="24"/>
       <c r="C262" s="7" t="s">
         <v>24</v>
       </c>
@@ -19919,7 +19919,7 @@
     </row>
     <row r="263" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A263" s="22"/>
-      <c r="B263" s="25"/>
+      <c r="B263" s="24"/>
       <c r="C263" s="7" t="s">
         <v>24</v>
       </c>
@@ -19992,7 +19992,7 @@
     </row>
     <row r="264" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A264" s="22"/>
-      <c r="B264" s="25"/>
+      <c r="B264" s="24"/>
       <c r="C264" s="7" t="s">
         <v>24</v>
       </c>
@@ -20065,7 +20065,7 @@
     </row>
     <row r="265" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A265" s="22"/>
-      <c r="B265" s="25"/>
+      <c r="B265" s="24"/>
       <c r="C265" s="7" t="s">
         <v>24</v>
       </c>
@@ -20138,7 +20138,7 @@
     </row>
     <row r="266" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A266" s="22"/>
-      <c r="B266" s="25"/>
+      <c r="B266" s="24"/>
       <c r="C266" s="7" t="s">
         <v>24</v>
       </c>
@@ -20211,7 +20211,7 @@
     </row>
     <row r="267" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A267" s="22"/>
-      <c r="B267" s="25"/>
+      <c r="B267" s="24"/>
       <c r="C267" s="7" t="s">
         <v>24</v>
       </c>
@@ -20284,7 +20284,7 @@
     </row>
     <row r="268" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A268" s="22"/>
-      <c r="B268" s="25"/>
+      <c r="B268" s="24"/>
       <c r="C268" s="7" t="s">
         <v>24</v>
       </c>
@@ -20357,7 +20357,7 @@
     </row>
     <row r="269" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A269" s="22"/>
-      <c r="B269" s="25"/>
+      <c r="B269" s="24"/>
       <c r="C269" s="7" t="s">
         <v>24</v>
       </c>
@@ -20430,7 +20430,7 @@
     </row>
     <row r="270" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A270" s="22"/>
-      <c r="B270" s="25"/>
+      <c r="B270" s="24"/>
       <c r="C270" s="7" t="s">
         <v>24</v>
       </c>
@@ -20503,7 +20503,7 @@
     </row>
     <row r="271" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A271" s="22"/>
-      <c r="B271" s="25"/>
+      <c r="B271" s="24"/>
       <c r="C271" s="7" t="s">
         <v>24</v>
       </c>
@@ -20576,7 +20576,7 @@
     </row>
     <row r="272" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A272" s="22"/>
-      <c r="B272" s="25"/>
+      <c r="B272" s="24"/>
       <c r="C272" s="7" t="s">
         <v>24</v>
       </c>
@@ -20649,7 +20649,7 @@
     </row>
     <row r="273" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A273" s="22"/>
-      <c r="B273" s="25"/>
+      <c r="B273" s="24"/>
       <c r="C273" s="7" t="s">
         <v>24</v>
       </c>
@@ -20722,7 +20722,7 @@
     </row>
     <row r="274" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A274" s="22"/>
-      <c r="B274" s="25"/>
+      <c r="B274" s="24"/>
       <c r="C274" s="7" t="s">
         <v>24</v>
       </c>
@@ -20795,7 +20795,7 @@
     </row>
     <row r="275" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A275" s="22"/>
-      <c r="B275" s="25"/>
+      <c r="B275" s="24"/>
       <c r="C275" s="7" t="s">
         <v>24</v>
       </c>
@@ -20868,7 +20868,7 @@
     </row>
     <row r="276" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A276" s="22"/>
-      <c r="B276" s="25"/>
+      <c r="B276" s="24"/>
       <c r="C276" s="7" t="s">
         <v>24</v>
       </c>
@@ -20941,7 +20941,7 @@
     </row>
     <row r="277" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A277" s="22"/>
-      <c r="B277" s="25"/>
+      <c r="B277" s="24"/>
       <c r="C277" s="7" t="s">
         <v>24</v>
       </c>
@@ -21014,7 +21014,7 @@
     </row>
     <row r="278" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A278" s="22"/>
-      <c r="B278" s="25"/>
+      <c r="B278" s="24"/>
       <c r="C278" s="7" t="s">
         <v>24</v>
       </c>
@@ -21087,7 +21087,7 @@
     </row>
     <row r="279" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A279" s="22"/>
-      <c r="B279" s="25"/>
+      <c r="B279" s="24"/>
       <c r="C279" s="7" t="s">
         <v>24</v>
       </c>
@@ -21160,7 +21160,7 @@
     </row>
     <row r="280" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A280" s="22"/>
-      <c r="B280" s="25"/>
+      <c r="B280" s="24"/>
       <c r="C280" s="7" t="s">
         <v>24</v>
       </c>
@@ -21233,7 +21233,7 @@
     </row>
     <row r="281" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A281" s="22"/>
-      <c r="B281" s="25"/>
+      <c r="B281" s="24"/>
       <c r="C281" s="7" t="s">
         <v>24</v>
       </c>
@@ -21306,7 +21306,7 @@
     </row>
     <row r="282" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A282" s="22"/>
-      <c r="B282" s="25"/>
+      <c r="B282" s="24"/>
       <c r="C282" s="7" t="s">
         <v>24</v>
       </c>
@@ -21379,7 +21379,7 @@
     </row>
     <row r="283" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A283" s="22"/>
-      <c r="B283" s="25"/>
+      <c r="B283" s="24"/>
       <c r="C283" s="7" t="s">
         <v>24</v>
       </c>
@@ -21452,7 +21452,7 @@
     </row>
     <row r="284" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A284" s="22"/>
-      <c r="B284" s="25"/>
+      <c r="B284" s="24"/>
       <c r="C284" s="7" t="s">
         <v>24</v>
       </c>
@@ -21525,7 +21525,7 @@
     </row>
     <row r="285" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A285" s="22"/>
-      <c r="B285" s="25"/>
+      <c r="B285" s="24"/>
       <c r="C285" s="7" t="s">
         <v>24</v>
       </c>
@@ -21598,7 +21598,7 @@
     </row>
     <row r="286" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A286" s="22"/>
-      <c r="B286" s="25"/>
+      <c r="B286" s="24"/>
       <c r="C286" s="7" t="s">
         <v>24</v>
       </c>
@@ -21671,7 +21671,7 @@
     </row>
     <row r="287" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A287" s="22"/>
-      <c r="B287" s="25"/>
+      <c r="B287" s="24"/>
       <c r="C287" s="7" t="s">
         <v>24</v>
       </c>
@@ -21744,7 +21744,7 @@
     </row>
     <row r="288" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A288" s="22"/>
-      <c r="B288" s="25"/>
+      <c r="B288" s="24"/>
       <c r="C288" s="7" t="s">
         <v>24</v>
       </c>
@@ -21817,7 +21817,7 @@
     </row>
     <row r="289" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A289" s="22"/>
-      <c r="B289" s="25"/>
+      <c r="B289" s="24"/>
       <c r="C289" s="7" t="s">
         <v>24</v>
       </c>
@@ -21890,7 +21890,7 @@
     </row>
     <row r="290" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A290" s="22"/>
-      <c r="B290" s="25"/>
+      <c r="B290" s="24"/>
       <c r="C290" s="7" t="s">
         <v>24</v>
       </c>
@@ -21963,7 +21963,7 @@
     </row>
     <row r="291" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A291" s="22"/>
-      <c r="B291" s="25"/>
+      <c r="B291" s="24"/>
       <c r="C291" s="7" t="s">
         <v>24</v>
       </c>
@@ -22036,7 +22036,7 @@
     </row>
     <row r="292" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A292" s="22"/>
-      <c r="B292" s="25"/>
+      <c r="B292" s="24"/>
       <c r="C292" s="7" t="s">
         <v>24</v>
       </c>
@@ -22109,7 +22109,7 @@
     </row>
     <row r="293" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A293" s="22"/>
-      <c r="B293" s="25"/>
+      <c r="B293" s="24"/>
       <c r="C293" s="7" t="s">
         <v>24</v>
       </c>
@@ -22182,7 +22182,7 @@
     </row>
     <row r="294" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A294" s="22"/>
-      <c r="B294" s="25"/>
+      <c r="B294" s="24"/>
       <c r="C294" s="7" t="s">
         <v>24</v>
       </c>
@@ -22255,7 +22255,7 @@
     </row>
     <row r="295" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A295" s="22"/>
-      <c r="B295" s="25"/>
+      <c r="B295" s="24"/>
       <c r="C295" s="7" t="s">
         <v>24</v>
       </c>
@@ -22328,7 +22328,7 @@
     </row>
     <row r="296" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A296" s="22"/>
-      <c r="B296" s="25"/>
+      <c r="B296" s="24"/>
       <c r="C296" s="7" t="s">
         <v>24</v>
       </c>
@@ -22401,7 +22401,7 @@
     </row>
     <row r="297" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A297" s="22"/>
-      <c r="B297" s="25"/>
+      <c r="B297" s="24"/>
       <c r="C297" s="7" t="s">
         <v>24</v>
       </c>
@@ -22474,7 +22474,7 @@
     </row>
     <row r="298" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A298" s="22"/>
-      <c r="B298" s="25"/>
+      <c r="B298" s="24"/>
       <c r="C298" s="7" t="s">
         <v>24</v>
       </c>
@@ -22547,7 +22547,7 @@
     </row>
     <row r="299" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A299" s="22"/>
-      <c r="B299" s="25"/>
+      <c r="B299" s="24"/>
       <c r="C299" s="7" t="s">
         <v>24</v>
       </c>
@@ -22620,8 +22620,8 @@
     </row>
     <row r="300" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A300" s="22"/>
-      <c r="B300" s="25"/>
-      <c r="C300" s="27" t="s">
+      <c r="B300" s="24"/>
+      <c r="C300" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D300" s="7" t="s">
@@ -22693,7 +22693,7 @@
     </row>
     <row r="301" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A301" s="23"/>
-      <c r="B301" s="26"/>
+      <c r="B301" s="25"/>
       <c r="C301" s="15" t="s">
         <v>24</v>
       </c>
@@ -22819,7 +22819,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection password="C0EF" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <customSheetViews>
     <customSheetView guid="{E33A81B8-4E62-4CEF-8E86-36C5209ED9BD}" scale="140">
       <selection activeCell="D15" sqref="A1:XFD1048576"/>

</xml_diff>